<commit_message>
Sử dụng docker stack chạy các dịch vụ trên swarm
</commit_message>
<xml_diff>
--- a/utb/chay-dich-vu-tren-docker-swarm/chay-dich-vu-tren-docker-swarm.xlsx
+++ b/utb/chay-dich-vu-tren-docker-swarm/chay-dich-vu-tren-docker-swarm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\source\docker\utb\chay-dich-vu-tren-docker-swarm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8901F9B2-9679-4B5F-A33E-B78621442682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA77E32-CF00-433B-BCCD-220B3DA3A5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="docker host and list node" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="106">
   <si>
     <t>sudo docker node ls</t>
   </si>
@@ -354,13 +354,16 @@
   </si>
   <si>
     <t>Thống kê lại các container trên vps3</t>
+  </si>
+  <si>
+    <t>Không cần pull image</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,13 +371,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -389,9 +405,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,7 +621,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>579962</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>142405</xdr:rowOff>
+      <xdr:rowOff>94780</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4149,7 +4167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2985BCD9-5BB1-4FA8-A69D-B4D29C165ABE}">
   <dimension ref="A2:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -4178,10 +4196,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE189294-FD83-442F-98D1-E7C67DFE090D}">
-  <dimension ref="A2:P188"/>
+  <dimension ref="A2:S188"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4196,42 +4214,1070 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+    </row>
+    <row r="38" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="2"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="2"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="2"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="R62" s="2"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="2"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2"/>
+      <c r="R64" s="2"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2"/>
+      <c r="R65" s="2"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="2"/>
+      <c r="Q66" s="2"/>
+      <c r="R66" s="2"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="2"/>
+      <c r="Q67" s="2"/>
+      <c r="R67" s="2"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="P75" s="1" t="s">
         <v>71</v>
       </c>
@@ -4338,7 +5384,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4346,8 +5393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D2A70F-8D9E-4805-AFE0-D123CC11985D}">
   <dimension ref="A2:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4703,7 +5750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AEB3105-F381-41F9-9C4E-15E34C85452D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
@@ -4963,7 +6010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B6A180-33EC-48A1-BC92-9856A4D267D7}">
   <dimension ref="A2:B96"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
@@ -5024,7 +6071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0778E19-0FDA-4ED3-B0D1-500D441A6CFD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>

</xml_diff>